<commit_message>
add Bare Point data
</commit_message>
<xml_diff>
--- a/data/data-inventory-matrix.xlsx
+++ b/data/data-inventory-matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor/SynologyDrive/Cisco-Climate-Change/Coregonine-Embryo-Modeling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6E9377-8769-EA43-BE8D-956A9E24DFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F241DDBC-D4C8-4747-BBAB-C3D8523F9AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{7D036444-8B42-0641-AB94-28DF609DF033}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30820" windowHeight="18440" xr2:uid="{7D036444-8B42-0641-AB94-28DF609DF033}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>lake</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>Eckmann, 1987</t>
+  </si>
+  <si>
+    <t>Luczyński &amp; Kirklewska, 1984</t>
+  </si>
+  <si>
+    <t>Colby &amp; Brooke, 1973</t>
+  </si>
+  <si>
+    <t>garda</t>
+  </si>
+  <si>
+    <t>?? Checking</t>
   </si>
 </sst>
 </file>
@@ -442,166 +454,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBFDD3BB-F63E-B84A-ADE4-BB6759605B67}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D10" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
-        <v>13</v>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust to using climate zones
</commit_message>
<xml_diff>
--- a/data/data-inventory-matrix.xlsx
+++ b/data/data-inventory-matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor/SynologyDrive/Cisco-Climate-Change/Coregonine-Embryo-Modeling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F241DDBC-D4C8-4747-BBAB-C3D8523F9AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE97AB7-FCD8-724A-A423-C2AD17C08D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30820" windowHeight="18440" xr2:uid="{7D036444-8B42-0641-AB94-28DF609DF033}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
   <si>
     <t>lake</t>
   </si>
@@ -78,9 +78,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>in process</t>
-  </si>
-  <si>
     <t>Dan?</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>?? Checking</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,21 +486,24 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -511,7 +514,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -520,7 +523,7 @@
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -534,7 +537,7 @@
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -547,8 +550,11 @@
       <c r="D5" t="s">
         <v>13</v>
       </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -559,7 +565,7 @@
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -579,7 +585,7 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -599,7 +605,7 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -619,7 +625,7 @@
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -630,16 +636,16 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>